<commit_message>
Created a proposal Memo and updated BOM
</commit_message>
<xml_diff>
--- a/Preliminary Proposal/ME 507 Project BOM.xlsx
+++ b/Preliminary Proposal/ME 507 Project BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reesv\Documents\School Stuff\Spring 2023\ME 507\Term Project\ME-507-Project\Preliminary Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reesv\Documents\School Stuff\Spring 2023\ME 507\ME-507-Project\Preliminary Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D77D7EA-575B-43CF-8AC9-DFFF19FC0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4521E6-9A5C-4754-893E-DD8F6B4F78F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{94A590EB-B9E5-4046-A1ED-3BCF3BF90D42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94A590EB-B9E5-4046-A1ED-3BCF3BF90D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Intake Motor</t>
   </si>
@@ -50,24 +72,12 @@
     <t>Line Sensor</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/dfrobot/FIT0186/6588528</t>
-  </si>
-  <si>
     <t>Drive Motors x 2</t>
   </si>
   <si>
     <t>Camera</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B08ML8QKPG/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;th=1</t>
-  </si>
-  <si>
-    <t>amazon.com/gp/product/B07MFK266B/ref=ppx_yo_dt_b_asin_title_o04_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/VEML3328/10673129</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/ROB-09454/5725749?utm_adgroup=Evaluation%20Boards%20-%20Sensors&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Development%20Boards%2C%20Kits%2C%20Programmers_NEW&amp;utm_term=&amp;utm_content=Evaluation%20Boards%20-%20Sensors&amp;gclid=CjwKCAjw8-OhBhB5EiwADyoY1VGQYtST6vz0AVjgcWqKBNPc5gkdeywf87u9AykjCNSaEk6VWj7bQRoCzAUQAvD_BwE</t>
   </si>
   <si>
@@ -96,6 +106,33 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/VEML3328/10673129 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/pololu-corporation/4824/10450234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/gp/product/B08ML8QKPG/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;th=1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/gp/product/B07MFK266B/ref=ppx_yo_dt_b_asin_title_o04_s00?ie=UTF8&amp;psc=1 </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -106,8 +143,24 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,15 +185,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,65 +512,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27220279-047C-4E44-AB7A-7C35712B983F}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -519,25 +588,31 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>47.45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -547,11 +622,14 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -561,11 +639,14 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -575,11 +656,14 @@
       <c r="C8" s="2">
         <v>2.77</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -589,13 +673,16 @@
       <c r="C9" s="2">
         <v>3.5</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -603,11 +690,36 @@
       <c r="C10" s="1">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" cm="1">
+        <f t="array" ref="C11">SUM(C2:C10*B2:B10)</f>
+        <v>156.17000000000002</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{141B8E32-3171-4B8D-9ABB-6E7E92647A5D}"/>
+    <hyperlink ref="E10" r:id="rId2" display="https://www.amazon.com/AITIAO-640x480-0-3Mega-Compatible-Interface/dp/B09QM3KTVK/ref=asc_df_B09QM3KTVK/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=632163229910&amp;hvpos=&amp;hvnetw=g&amp;hvrand=1079724021006747850&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1014232&amp;hvtargid=pla-1879959436542&amp;psc=1" xr:uid="{CAE5ED19-38E0-4391-AAE7-53744D29D339}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{15FE52EE-886D-438D-9D44-28ACBD473C00}"/>
+    <hyperlink ref="E9" r:id="rId4" display="https://www.digikey.com/en/products/detail/sparkfun-electronics/ROB-09454/5725749?utm_adgroup=Evaluation%20Boards%20-%20Sensors&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Development%20Boards%2C%20Kits%2C%20Programmers_NEW&amp;utm_term=&amp;utm_content=Evaluation%20Boards%20-%20Sensors&amp;gclid=CjwKCAjw8-OhBhB5EiwADyoY1VGQYtST6vz0AVjgcWqKBNPc5gkdeywf87u9AykjCNSaEk6VWj7bQRoCzAUQAvD_BwE" xr:uid="{52DA999E-2C65-471B-AD42-51156A1FD96F}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{5BF347BB-BE17-4C59-8626-0AE1DC834764}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{03FFF87F-59FB-4E8D-A764-28C968420AAF}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{36DFEF2F-2143-4298-BA73-284DD4A5C24B}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{A23F635B-1587-422C-821D-BC21B898AF9C}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{E5CDD467-03E6-4DC7-A4CF-AD134E7EF4C3}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{94FDDDC2-6906-43AF-A3F9-A35BE152552D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>